<commit_message>
Updated report with screenshots etc.
</commit_message>
<xml_diff>
--- a/Data Gathered and Results/Test #3 Elitism (4,10,20 Percent)/Results.xlsx
+++ b/Data Gathered and Results/Test #3 Elitism (4,10,20 Percent)/Results.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark\git\SET10107Coursework\Data Gathered and Results\Test #3 Elitism (4,10,20 Percent)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\git\SET10107Coursework\Data Gathered and Results\Test #3 Elitism (4,10,20 Percent)\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12870" yWindow="0" windowWidth="16065" windowHeight="11610"/>
+    <workbookView xWindow="13824" yWindow="0" windowWidth="16068" windowHeight="11616"/>
   </bookViews>
   <sheets>
     <sheet name="Initial benchmark" sheetId="1" r:id="rId1"/>
@@ -151,6 +151,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -628,7 +631,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -642,6 +645,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -894,7 +898,7 @@
               </c:extLst>
               <c:f>('Initial benchmark'!$C$33:$F$33,'Initial benchmark'!$I$33:$L$33,'Initial benchmark'!$O$33:$Q$33)</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.000000000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>5.7377994636172408E-2</c:v>
@@ -1037,7 +1041,7 @@
               </c:extLst>
               <c:f>('Initial benchmark'!$C$34:$F$34,'Initial benchmark'!$I$34:$L$34,'Initial benchmark'!$O$34:$Q$34)</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.000000000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>1.7566111812234126E-2</c:v>
@@ -1180,7 +1184,7 @@
               </c:extLst>
               <c:f>('Initial benchmark'!$C$35:$F$35,'Initial benchmark'!$I$35:$L$35,'Initial benchmark'!$O$35:$Q$35)</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.000000000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>3.5575207531043374E-2</c:v>
@@ -1323,7 +1327,7 @@
               </c:extLst>
               <c:f>('Initial benchmark'!$C$36:$F$36,'Initial benchmark'!$I$36:$L$36,'Initial benchmark'!$O$36:$Q$36)</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.000000000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>3.936889891736315E-2</c:v>
@@ -1466,7 +1470,7 @@
               </c:extLst>
               <c:f>('Initial benchmark'!$C$37:$F$37,'Initial benchmark'!$I$37:$L$37,'Initial benchmark'!$O$37:$Q$37)</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.000000000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>3.7866347907153153E-2</c:v>
@@ -1609,7 +1613,7 @@
               </c:extLst>
               <c:f>('Initial benchmark'!$C$38:$F$38,'Initial benchmark'!$I$38:$L$38,'Initial benchmark'!$O$38:$Q$38)</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.000000000</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>3.7077758541253378E-2</c:v>
@@ -4011,15 +4015,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>171449</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:colOff>650420</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>75520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>152399</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>21770</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4346,28 +4350,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F55" workbookViewId="0">
-      <selection activeCell="I89" sqref="I89"/>
+    <sheetView tabSelected="1" topLeftCell="F58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="32.140625" customWidth="1"/>
-    <col min="8" max="8" width="33.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="41.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" customWidth="1"/>
+    <col min="7" max="7" width="32.109375" customWidth="1"/>
+    <col min="8" max="8" width="33.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="13" max="13" width="29.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="13" max="13" width="29.44140625" customWidth="1"/>
     <col min="14" max="14" width="23" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" customWidth="1"/>
+    <col min="16" max="16" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4399,7 +4404,7 @@
       </c>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4431,7 +4436,7 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -4463,7 +4468,7 @@
       </c>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -4495,7 +4500,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -4528,7 +4533,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -4560,7 +4565,7 @@
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -4592,7 +4597,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -4624,7 +4629,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -4653,7 +4658,7 @@
         <v>2.4967642049836199E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -4682,7 +4687,7 @@
         <v>3.2557289032429703E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -4711,7 +4716,7 @@
         <v>2.60531727543509E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -4740,7 +4745,7 @@
         <v>2.8194267781994902E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -4769,7 +4774,7 @@
         <v>2.4641734863808998E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -4798,7 +4803,7 @@
         <v>3.2662533931226197E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -4827,7 +4832,7 @@
         <v>2.7589602067690001E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -4856,7 +4861,7 @@
         <v>3.0701448433839902E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -4885,7 +4890,7 @@
         <v>7.2690253678456399E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -4914,7 +4919,7 @@
         <v>0.15688681604372701</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -4943,7 +4948,7 @@
         <v>6.5670964704373003E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -4972,7 +4977,7 @@
         <v>0.15497362955592101</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -5001,7 +5006,7 @@
         <v>6.3045207192645794E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -5030,7 +5035,7 @@
         <v>0.18099943530056101</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -5059,7 +5064,7 @@
         <v>6.4840141646496097E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -5088,7 +5093,7 @@
         <v>0.15407331003017999</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -5099,7 +5104,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -5110,7 +5115,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -5121,7 +5126,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -5132,7 +5137,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -5143,7 +5148,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -5154,7 +5159,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C31" s="6" t="s">
         <v>27</v>
       </c>
@@ -5171,7 +5176,7 @@
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
         <v>0</v>
       </c>
@@ -5200,7 +5205,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -5211,7 +5216,7 @@
         <f>AVERAGE(C2,C4,C6,C8)</f>
         <v>5.7377994636172408E-2</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="7">
         <f>AVERAGE(C10,C12,C14,C16)</f>
         <v>2.7864278204276925E-4</v>
       </c>
@@ -5229,7 +5234,7 @@
         <f>AVERAGE(I2,I4,I6,I8)</f>
         <v>5.5541044889306848E-2</v>
       </c>
-      <c r="J33" s="1">
+      <c r="J33" s="7">
         <f>AVERAGE(I10,I12,I14,I16)</f>
         <v>3.1432020799665152E-4</v>
       </c>
@@ -5247,7 +5252,7 @@
         <f>AVERAGE(O2,O4,O6,O8)</f>
         <v>5.6980163284618496E-2</v>
       </c>
-      <c r="P33" s="1">
+      <c r="P33" s="7">
         <f>AVERAGE(O10,O12,O14,O16)</f>
         <v>3.1028884794872679E-4</v>
       </c>
@@ -5256,7 +5261,7 @@
         <v>0.16173329773259726</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>12</v>
       </c>
@@ -5264,7 +5269,7 @@
         <f>AVERAGE(C1,C3,C5,C7)</f>
         <v>1.7566111812234126E-2</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="7">
         <f>AVERAGE(C9,C11,C13,C15)</f>
         <v>2.1047126777831851E-5</v>
       </c>
@@ -5279,7 +5284,7 @@
         <f>AVERAGE(I1,I3,I5,I7)</f>
         <v>1.6915469775438775E-2</v>
       </c>
-      <c r="J34" s="1">
+      <c r="J34" s="7">
         <f>AVERAGE(I9,I11,I13,I15)</f>
         <v>2.3848658253277152E-5</v>
       </c>
@@ -5294,7 +5299,7 @@
         <f>AVERAGE(O1,O3,O5,O7)</f>
         <v>1.73225694773264E-2</v>
       </c>
-      <c r="P34" s="1">
+      <c r="P34" s="7">
         <f>AVERAGE(O9,O11,O13,O15)</f>
         <v>2.5813037933921526E-5</v>
       </c>
@@ -5303,7 +5308,7 @@
         <v>6.6561641805492816E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -5314,7 +5319,7 @@
         <f>AVERAGE(C1,C2,C3,C4)</f>
         <v>3.5575207531043374E-2</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="7">
         <f>AVERAGE(C9,C10,C11,C12)</f>
         <v>1.4124712728596351E-4</v>
       </c>
@@ -5332,7 +5337,7 @@
         <f>AVERAGE(I1,I2,I3,I4)</f>
         <v>3.6835158485267902E-2</v>
       </c>
-      <c r="J35" s="1">
+      <c r="J35" s="7">
         <f>AVERAGE(I9,I10,I11,I12)</f>
         <v>1.7654298876948601E-4</v>
       </c>
@@ -5350,7 +5355,7 @@
         <f>AVERAGE(O1,O2,O3,O4)</f>
         <v>3.7755658957022376E-2</v>
       </c>
-      <c r="P35" s="1">
+      <c r="P35" s="7">
         <f>AVERAGE(O9,O10,O11,O12)</f>
         <v>1.6463409573710827E-4</v>
       </c>
@@ -5359,7 +5364,7 @@
         <v>0.11255541599561936</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>18</v>
       </c>
@@ -5367,7 +5372,7 @@
         <f>AVERAGE(C5,C6,C7,C8)</f>
         <v>3.936889891736315E-2</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="7">
         <f>AVERAGE(C13,C14,C15,C16)</f>
         <v>1.5844278153463758E-4</v>
       </c>
@@ -5382,7 +5387,7 @@
         <f>AVERAGE(I5,I6,I7,I8)</f>
         <v>3.5621356179477724E-2</v>
       </c>
-      <c r="J36" s="1">
+      <c r="J36" s="7">
         <f>AVERAGE(I13,I14,I15,I16)</f>
         <v>1.6162587748044265E-4</v>
       </c>
@@ -5397,7 +5402,7 @@
         <f>AVERAGE(O5,O6,O7,O8)</f>
         <v>3.6547073804922524E-2</v>
       </c>
-      <c r="P36" s="1">
+      <c r="P36" s="7">
         <f>AVERAGE(O13,O14,O15,O16)</f>
         <v>1.7146779014554E-4</v>
       </c>
@@ -5406,7 +5411,7 @@
         <v>0.11573952354247072</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -5417,7 +5422,7 @@
         <f>AVERAGE(C1,C4,C5,C8)</f>
         <v>3.7866347907153153E-2</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37" s="7">
         <f>AVERAGE(C9,C12,C13,C16)</f>
         <v>1.4686097302385264E-4</v>
       </c>
@@ -5435,7 +5440,7 @@
         <f>AVERAGE(I1,I4,I5,I8)</f>
         <v>3.8019563972000375E-2</v>
       </c>
-      <c r="J37" s="1">
+      <c r="J37" s="7">
         <f>AVERAGE(I9,I12,I13,I16)</f>
         <v>1.7982007995041757E-4</v>
       </c>
@@ -5453,7 +5458,7 @@
         <f>AVERAGE(O1,O4,O5,O8)</f>
         <v>3.7279211312868675E-2</v>
       </c>
-      <c r="P37" s="1">
+      <c r="P37" s="7">
         <f>AVERAGE(O9,O12,O13,O16)</f>
         <v>1.5964163476799831E-4</v>
       </c>
@@ -5462,7 +5467,7 @@
         <v>0.1111956001143008</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>17</v>
       </c>
@@ -5470,7 +5475,7 @@
         <f>AVERAGE(C2,C3,C6,C7)</f>
         <v>3.7077758541253378E-2</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="7">
         <f>AVERAGE(C10,C11,C14,C15)</f>
         <v>1.5282893579674845E-4</v>
       </c>
@@ -5485,7 +5490,7 @@
         <f>AVERAGE(I2,I3,I6,I7)</f>
         <v>3.4436950692745244E-2</v>
       </c>
-      <c r="J38" s="1">
+      <c r="J38" s="7">
         <f>AVERAGE(I10,I11,I14,I15)</f>
         <v>1.5834878629951109E-4</v>
       </c>
@@ -5500,7 +5505,7 @@
         <f>AVERAGE(O2,O3,O6,O7)</f>
         <v>3.7023521449076224E-2</v>
       </c>
-      <c r="P38" s="1">
+      <c r="P38" s="7">
         <f>AVERAGE(O10,O11,O14,O15)</f>
         <v>1.7646025111464999E-4</v>
       </c>
@@ -5509,12 +5514,12 @@
         <v>0.11709933942378928</v>
       </c>
     </row>
-    <row r="79" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I79" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="80" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I80" s="4" t="s">
         <v>32</v>
       </c>
@@ -5525,7 +5530,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H81" t="s">
         <v>34</v>
       </c>
@@ -5539,7 +5544,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="82" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H82" t="s">
         <v>35</v>
       </c>
@@ -5553,7 +5558,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="83" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H83" t="s">
         <v>36</v>
       </c>
@@ -5567,7 +5572,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="84" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H84" t="s">
         <v>37</v>
       </c>
@@ -5581,7 +5586,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="85" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H85" t="s">
         <v>38</v>
       </c>
@@ -5595,7 +5600,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="86" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H86" t="s">
         <v>39</v>
       </c>
@@ -5609,7 +5614,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="87" spans="8:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H87" s="2" t="s">
         <v>41</v>
       </c>

</xml_diff>